<commit_message>
Complete working bs4 scraping with sort.
</commit_message>
<xml_diff>
--- a/data_mining/bikes.xlsx
+++ b/data_mining/bikes.xlsx
@@ -452,1721 +452,1549 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Avenue spirit 1000</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
+          <t>Степенка за велосипед</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/10/fp/106de41fa4f6c84eaa01448a0a5abbf1.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/d7/fp/d7ed5717b397a30e15b330a037cb183b.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>велосипед 26 цола CONWAY-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>155</t>
-        </is>
+          <t>Гуми 28 цола nimbus700×32c kenda цената е за 2-те гуми</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>25</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/d2/fp/d2c10a8fca2b11b86fdffcc0b316cf6c.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//da/fp/da81f5744ca833b088bbbfd2118af84e.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+          <t>Калъф стойка за телефон монтаж за колело</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/61/fp/61c5ca62cd6a1d83f1eb01b82fedad4a.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//86/fp/861f50d5ecccf43f34e7b9b664224ac8.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>велосипед Cannondale USA</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+          <t>Две капли 26” оборудвани с гуми + бонус</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>55</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/33/fp/338062f566da65f604a110e8f9be9b2f.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/5f/fp/5f43794ab809428bb372a605143f005f.jpg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Велосипед Ultra phantom 26 цола</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
+          <t>Детски велосипед 16 цола - разпродажба</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>69</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/97/fp/9714505365f2f0451f592fd814215f8d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/4b/fp/4b6361302ca61368c0a67ae05c12ffec.jpg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД SHIMANO BIKE 28-ЦОЛА</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>рамка 52см и вилка (феникс 28")</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>70</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/d5/fp/d5800a602d4e2aa2f0e41acd0b9dac3a.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/8d/fp/8d88b108c0cc43251b3b56a682942e3b.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Градски велосипед 28цола</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+          <t>Велосипед Pegasus</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>75</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/18/fp/18a5dc836f65140ee46f3e7ac76e9b96.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//79/fp/7901eea28bb025a074d260e815daa888.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Велосипед интербайк</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>85</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/b0/fp/b0d25327a0c7e2aaf5da2b27ed97a0cd.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/4b/fp/4b54e94ea3ca6ca1c5dcb9057a63a1e9.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kross commuter велосипед</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>180</t>
-        </is>
+          <t>20цолов велосипед Calypso с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>89</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/e1/fp/e16cd61a2dad5cb0497d72589373d0ab.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/17/fp/179ac9264931faa480b302fc92bc810e.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед/колело B-Twin 26"</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>290</t>
-        </is>
+          <t>18цолов велосипед BMX Wicked с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>89</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/8b/fp/8b95cfde68e60f75bd68a79369eeda8c.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/5b/fp/5bd3d28ea6d6209f4e2b41256d2e16c1.jpg</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>137</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ел. колело, електрическо колело, електро колело</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>90</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//42/fp/4205ae8e47ce0f1e05d60ddbfc015098.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/99/fp/99319cb3fe4ad0c112f975d6ec23f2fc.jpg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>"Марлин" алуминий,26"на2.10 оборудвано,реновирано</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>180</t>
-        </is>
+          <t>18цолов детски велосипед с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>99</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/dc/fp/dc9efe684e58eb88f293564d62b3d7c0.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/5c/fp/5c653da616a5ad68ce0e8ea9ac2c3e1d.jpg</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Продавам Градски Велосипед Sprint Elegance 28 ''</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>18цолов детски велосипед с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>99</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/d9/fp/d94b8799c02289a1837f089152a186a5.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/5c/fp/5c653da616a5ad68ce0e8ea9ac2c3e1d.jpg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>180</t>
-        </is>
+          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>99</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/3e/fp/3e6c13f3c21687bd61e84d73d3a89785.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Продавам алуминиев велосипед 26"</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>99</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/15/fp/151329c21953a1b5229d546b1f38510b.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Велосипед/колело Cross Alissa 24</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>110</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/c4/fp/c4adf41ce34b6974db077c1fe693a6eb.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/60/fp/60a697db700ce2a22d751a4dc7873d5b.jpg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>велосипед градски</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД KALKHOFF CITY SHOPPER</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>110</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/9d/fp/9dedc9c9f80b2b2c3f62ff1857ff3540.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/43/fp/439cd9eb0022a867012967a50072b928.jpg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Продавам немски велосипед</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>190</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД SHIMANO ROBIFIR</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>110</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/c9/fp/c9b5f5068212ff6c11cafc8d8c84f2f1.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/fc/fp/fc049c0828bd9602026f355d6e7f9b4f.jpg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Градски велосипед</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+          <t>Велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>120</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/8b/fp/8b79fac85cd3abde9b9057ed733d6c0d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/58/fp/5835a0a7be423ccd6c0be54132bc99bd.jpg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>octane one street dirt jump bike</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>120</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/c3/fp/c3c20bd0d19b39fe50739f83ad0c4ac9.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/cf/fp/cfc09ed8820b74624a56f668d99f1129.jpg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Колело 24 инча</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>185</t>
-        </is>
+          <t>Велосипед Vortex</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>120</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/c9/fp/c98a2cb66c65bff163bff79b0c241b49.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/55/fp/55ae897248b04f1fc652aec5b6e58530.jpg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Велосипед Pegasus</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+          <t>Продавам 20" велосипед Спринт, намалям на 110лв</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>120</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//79/fp/7901eea28bb025a074d260e815daa888.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/a5/fp/a52796afd563f6e0b61407e3f1ab7330.jpg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Велосипед Carratec</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Градски велосипед</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>120</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/29/fp/294c10a4f7dbb1b3306f65b84e679923.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/92/fp/927cc7e4970fe1b81dc2f56af6d90191.jpg</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Велосипед Nirve Fairfaxт</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>120</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//59/fp/592cd39b171d5836c336b79f324a2a17.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7e/fp/7e03101e7a579bba4d972136a89ab198.jpg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>рамка 52см и вилка (феникс 28")</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>130</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/8d/fp/8d88b108c0cc43251b3b56a682942e3b.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+          <t>Колело</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>130</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7e/fp/7e03101e7a579bba4d972136a89ab198.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/1f/fp/1fd32f2ae2d921744180a3ce13eab001.jpg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Продавам запазено колело</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>Продавам 2 бр. Велосипеди</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>130</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/18/fp/18420ba888752d14fdf6702dfc30d380.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18цолов велосипед BMX Wicked с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+          <t>Продавам 2 бр. Велосипеди</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>130</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/5b/fp/5bd3d28ea6d6209f4e2b41256d2e16c1.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
+          <t>Продавам 2 бр. Велосипеди</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>130</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/85/fp/85cb90dd4c1e76ce5611dd3d371e804e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
+        <v>148</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3 броя Велосипеди</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>18цолов велосипед Lark с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>130</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/71/fp/713a3ef09657d59f3d1889a5d8f40644.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/62/fp/62cb140e5648916e2d4d5aa99b2bfa56.jpg</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Детски велосипед 16 цола - разпродажба</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+          <t>Велосипед Carratec</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>130</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/4b/fp/4b6361302ca61368c0a67ae05c12ffec.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/29/fp/294c10a4f7dbb1b3306f65b84e679923.jpg</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Дамски велосипед DINLOP 28"</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+          <t>Колело</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>130</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/b4/fp/b4cd650b7286514a51f580004849fea2.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/b5/fp/b554b51321901354c708ddb02bfdeaea.jpg</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ГОЛЯМ ИЗБОР НА ВЕЛОСИПЕДИ, ДИСПЛЕИ,ЗАРЯДНИ,БАТЕРИИ И ДР.ЗА ЕЛЕКТРИЧЕСКИ ВЕЛОСИПЕДИ</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>Велосипед 24 цола Raleigh Ascender</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>135</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//e3/fp/e372d75b8bd2adde6a85f31fcb04e1f6.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/30/fp/306fae5cf84d2a1a423998655fe1fd0a.jpg</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Xiaomi M365 Гуми външни,вътрешни и плътни 8 1/2 х 2 Високо качество!</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+          <t>Велосипед "CAPRI"-Италия</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>140</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/10/fp/102f0aaa28d8eeb233f9db70f354d4e9.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/04/fp/0425dea5fc04328f726317e8754c578e.jpg</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Детско колело 16 цола Детски велосипед, Алуминиево колело, Алуминиев велосипед с дискови спирачки</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>349</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД PEGASUS 26-ЦОЛА</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>140</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/62/fp/62fb038769d2d37c057af55434456700.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/f1/fp/f1378a2509eff0d627d615333db0af41.jpg</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Велосипед Culture 26</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>190</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>145</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/89/fp/89dba8f29445e56a78603ef9f13ed4c4.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/db/fp/db2efb18d1df50251ab6d9ecdcdfd4d3.jpg</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Велосипед Releigh Void 24 цола</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>175</t>
-        </is>
+          <t>27цолов велосипед RALEIGH с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>149</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/e9/fp/e91e873c69baf06ba8a308e883e2d0c3.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/88/fp/885add0c17e1b14f6fcc05497e8c3012.jpg</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола KALKHOFF-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>420</t>
-        </is>
+          <t>Колело</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>150</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/82/fp/82a0641a95ee4309e7b96e769fce251b.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/3b/fp/3be430105cef4b14604676d018662d15.jpg</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>велосипед 24 цола BELLINI-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>175</t>
-        </is>
+          <t>Продавам велосипед СПЕШНО!!!</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>150</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/27/fp/27130043bc5e2743ee1ae2cd9c3dc361.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/82/fp/82cf4bedc46273f49494f4ddc7732654.jpg</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Продавам колело</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>160</t>
-        </is>
+          <t>Продавам Градски Велосипед Sprint Elegance 28 ''</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>150</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/07/fp/076f666a501190a067dd91b894302c8d.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/d9/fp/d94b8799c02289a1837f089152a186a5.jpg</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Степенка за велосипед</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+          <t>Велосипед/колело Cross Alissa 24</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>150</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/d7/fp/d7ed5717b397a30e15b330a037cb183b.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/c4/fp/c4adf41ce34b6974db077c1fe693a6eb.jpg</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Колело</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>Велосипед интербайк</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>150</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/3b/fp/3be430105cef4b14604676d018662d15.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/b0/fp/b0d25327a0c7e2aaf5da2b27ed97a0cd.jpg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Велосипед Appollo X Rated Jump 24 цола</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>180</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД SHIMANO BIKE 28-ЦОЛА</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>150</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7d/fp/7de807a473af9fca959deefaaf4c37ad.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/d5/fp/d5800a602d4e2aa2f0e41acd0b9dac3a.jpg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Колело miutin 26”</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+          <t>3 броя Велосипеди</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>150</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/92/fp/9206f82ee0561a90e053590f484a1926.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/71/fp/713a3ef09657d59f3d1889a5d8f40644.jpg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Немски електрически велосипед Kreidler 28</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+          <t>велосипед 26 цола CONWAY-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>155</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/c2/fp/c2d17836e616d2cd4120dcbfa1f9e4a1.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/d2/fp/d2c10a8fca2b11b86fdffcc0b316cf6c.jpg</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед Bulls 29</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+          <t>Продавам колело</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>160</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/46/fp/46dddbdc55bf343f74ca15663d4fff1c.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/07/fp/076f666a501190a067dd91b894302c8d.jpg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола PEGASUS-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>Класически велосипед SCOTT</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>160</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/28/fp/28f42ca8251736768a600fac96f37ed2.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/79/fp/79aeeb1a245196ccb6a15f3739b941c9.jpg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Колело</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Велосипед Gemini Outrider</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>160</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/b5/fp/b554b51321901354c708ddb02bfdeaea.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/0c/fp/0c5258b46ca3689f6fbc05bfb21e6648.jpg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Колело SERIOUS. ROCKVILE. 27,5 “. Рамка L.  27 ск.</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>580</t>
-        </is>
+          <t>Велосипед градски OBIKE-26цола.Бартер.</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>160</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/e5/fp/e58ef5fe4728d5855318b7e3f0abe3c2.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/e5/fp/e5c1468f5a90799fa452afa307596e70.jpg</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Колело</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Страхотен велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>160</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/1f/fp/1fd32f2ae2d921744180a3ce13eab001.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/4e/fp/4e44dd70c0403518b9ce49be0beb8b84.jpg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Велосипед Cannondele</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>680</t>
-        </is>
+          <t>велосипед 28 цола WINORA-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>165</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/a6/fp/a69ea0a8fb5b84dd62bdc65560b9a5f4.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/11/fp/11217cfc400f57e39e595737e40736c5.jpg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Велосипед Specialised</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+          <t>Велосипед Ultra phantom 26 цола</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>170</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/b1/fp/b1b54305233d78dedb6f96d170c89ad0.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/97/fp/9714505365f2f0451f592fd814215f8d.jpg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Велосипед 26цола 175лв</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>175</t>
-        </is>
+          <t>Велосипед Releigh Void 24 цола</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>175</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/e7/fp/e7cbd353be1d93c67fd7bfdac20e3051.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/e9/fp/e91e873c69baf06ba8a308e883e2d0c3.jpg</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола CONWAY-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>245</t>
-        </is>
+          <t>Велосипед 26цола 175лв</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>175</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/9b/fp/9b9b98eb2eebca958e31bfb51200a258.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/e7/fp/e7cbd353be1d93c67fd7bfdac20e3051.jpg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>велосипед 28 цола WINORA-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>165</t>
-        </is>
+          <t>велосипед 24 цола BELLINI-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>175</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/11/fp/11217cfc400f57e39e595737e40736c5.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/27/fp/27130043bc5e2743ee1ae2cd9c3dc361.jpg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Велосипед Vortex</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+          <t>Велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>180</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/55/fp/55ae897248b04f1fc652aec5b6e58530.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/3e/fp/3e6c13f3c21687bd61e84d73d3a89785.jpg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Градско колело City bike. 28”. Shimano 28 скорости</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+          <t>"Марлин" алуминий,26"на2.10 оборудвано,реновирано</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>180</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/65/fp/655c66aa98f01c32366e7002405175bd.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/dc/fp/dc9efe684e58eb88f293564d62b3d7c0.jpg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Велосипед хибрид Giant roam xr 2</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+          <t>Kross commuter велосипед</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>180</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/b9/fp/b9f9e4dc28d611b80ab8b03c6b4883dc.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/e1/fp/e16cd61a2dad5cb0497d72589373d0ab.jpg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Велосипед DRAG</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>Велосипед Appollo X Rated Jump 24 цола</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>180</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/2a/fp/2ae03f688c9a32660b819d0492d8e2ab.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7d/fp/7de807a473af9fca959deefaaf4c37ad.jpg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД СГЪВАЕМ B-TWIN TILT 120 20-ЦОЛА</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>295</t>
-        </is>
+          <t>Колело 24 инча</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>185</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/2b/fp/2bf8abbf86bcb0c01bc6d3b9b8fba539.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/c9/fp/c98a2cb66c65bff163bff79b0c241b49.jpg</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД ELECTRA LOFT 7D 2020г. модел 28-цола</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>540</t>
-        </is>
+          <t>Дамски велосипед Releigh M 290 24 цола</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>185</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/6b/fp/6badad64d8946a06936635cc00e8e959.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/8d/fp/8d6215ef89d665bb95f0d6bf1f3d99f8.jpg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД PEGASUS 26-ЦОЛА</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>140</t>
-        </is>
+          <t>велосипед 28 цола McKenzie-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>190</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/f1/fp/f1378a2509eff0d627d615333db0af41.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/67/fp/6772c2dc007c8981ffeaa7f01b6bdf8f.jpg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД NERO 28-ЦОЛА</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+          <t>Велосипед Culture 26</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>190</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/49/fp/498e5bbc3285f736fb5baf2dbfef62fc.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/89/fp/89dba8f29445e56a78603ef9f13ed4c4.jpg</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД B-TWIN ORIGINAL 500</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>270</t>
-        </is>
+          <t>Продавам немски велосипед</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>190</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/48/fp/4803796e9f073bc9bd1b09e9fbfeac8a.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/c9/fp/c9b5f5068212ff6c11cafc8d8c84f2f1.jpg</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД RIVERSIDE CIVERSIDE 320TR</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>390</t>
-        </is>
+          <t>Дамски велосипед DINLOP 28"</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>199</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7e/fp/7ea34bead5088898bc142cf5bd8f6b98.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/b4/fp/b4cd650b7286514a51f580004849fea2.jpg</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Карбонов велосипед  Specialized tarmac. 28 цола</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
+          <t>Велосипед мъжки 26" LEADER WILD CAR</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>200</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/24/fp/2496e26ad1d456b890fedf9813cc9731.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/32/fp/322552ed96a9c32c2e37371b81ac0525.jpg</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Градски алуминиев велосипед Ridgeback</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>200</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/b7/fp/b7712206a87e3c89b223b0c73919278d.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/19/fp/1991938570061c13cbb62b022c3d9d80.jpg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед GT 26 цола</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>БМХ</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>200</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/64/fp/64750510fd365eff6930a011c2e2e3f2.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/e4/fp/e41a52ce5b8f56dc892f87c7e0d51e6e.jpg</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Велосипед Rhino 24 цола</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>Колело Батавус</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>200</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/95/fp/953d69a058ee1a5e148674a122296ca0.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/be/fp/beb7a45e4b4d8bf5f24673c2f48e29c3.jpg</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Английски алуминиев велосипед  Appollo FS26</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
+          <t>велосипед градски</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>210</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/f3/fp/f3bd79150713f68df0eaca9293588ab7.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/9d/fp/9dedc9c9f80b2b2c3f62ff1857ff3540.jpg</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+          <t>Велосипед САРАЦЕН Роял</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>215</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/19/fp/1991938570061c13cbb62b022c3d9d80.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/d6/fp/d6590de5704d3ee70c528241a4ff0f78.jpg</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>145</t>
-        </is>
+          <t>Алуминиев велосипед GT 26 цола</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>220</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/db/fp/db2efb18d1df50251ab6d9ecdcdfd4d3.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/64/fp/64750510fd365eff6930a011c2e2e3f2.jpg</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола HERCULES-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>360</t>
-        </is>
+          <t>Дан Хил Велосипед Giant Box Three</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>220</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/fb/fp/fb0589b6a874359f72054b018e4c09ea.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/44/fp/443ec0dfa7302337885def175973ec1a.jpg</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+          <t>Колело Pegasus 26”, 21  скорости</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>220</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/cf/fp/cfc09ed8820b74624a56f668d99f1129.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/ab/fp/ab233c383eb90dc948c5d92e9f016c68.jpg</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Електрически велосипед</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
+          <t>Велосипед DRAG</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>220</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/53/fp/53983b72a173eb96188041242f3c00ed.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/2a/fp/2ae03f688c9a32660b819d0492d8e2ab.jpg</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Дамски велосипед Releigh M 290 24 цола</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>185</t>
-        </is>
+          <t>градски велосипед</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>220</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/8d/fp/8d6215ef89d665bb95f0d6bf1f3d99f8.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/9d/fp/9dedc9c9f80b2b2c3f62ff1857ff3540.jpg</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Американски велосипед GT ARROWHEAD</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+          <t>Дан Хил Велосипед Giant Box Three</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>220</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/52/fp/52b2be2c1f2ba2866d8450f1e719585b.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/8e/fp/8e3de7e8f6d2399ed729ea4b4ec5c218.jpg</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Туристически сгъваем велосипед Appollo Tuck 20цола</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
+          <t>Велосипед Rhino 24 цола</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>220</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/1c/fp/1c106e19bfa96317904bf0ed3ccba93c.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/95/fp/953d69a058ee1a5e148674a122296ca0.jpg</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Велосипед "CAPRI"-Италия</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>140</t>
-        </is>
+          <t>Btwin rockrider 25"</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>230</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/04/fp/0425dea5fc04328f726317e8754c578e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7f/fp/7fadf77edfc1059ddb6886bc3c1e0973.jpg</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД SHIMANO ROBIFIR</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+          <t>велосипед 28 цола VERDE-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>230</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/fc/fp/fc049c0828bd9602026f355d6e7f9b4f.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/15/fp/150553052dd810f9026dc425104c271e.jpg</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>велосипед 28 цола VERDE-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>230</t>
-        </is>
+          <t>Велосипед Apollo Rich 26 цола</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>240</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/15/fp/150553052dd810f9026dc425104c271e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/39/fp/39e1c1a38c1afc1b4930dd0ab31bd219.jpg</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола CALIFORNIA-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
+          <t>Туристически сгъваем велосипед Appollo Tuck 20цола</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>240</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/65/fp/6578e95773650636f181f828f29b110e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/1c/fp/1c106e19bfa96317904bf0ed3ccba93c.jpg</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>велосипед 28 цола McKenzie-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>190</t>
-        </is>
+          <t>Велосипед Аполо Рефлекс/ Apolo Reflex 20 цола</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>240</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/67/fp/6772c2dc007c8981ffeaa7f01b6bdf8f.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7c/fp/7c11da05fa04a8546bf3a713f2f6d474.jpg</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Продавам велосипед Рокрайдер с подобрения</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+          <t>алуминиев велосипед 28 цола CONWAY-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>245</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/0b/fp/0b8a549d0950aa4039e917a608cd60af.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/9b/fp/9b9b98eb2eebca958e31bfb51200a258.jpg</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Продавам велосипед СПЕШНО!!!</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
+          <t>Продавам велосипед Ultra PHANTOM/отлично състояние/ – купи до 31 август с 15% отстъпка</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>249</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/82/fp/82cf4bedc46273f49494f4ddc7732654.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/cf/fp/cf2dd9106d988f2d4c4444e227302206.jpg</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>БМХ</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+          <t>Продавам велосипед Ultra PHANTOM/отлично състояние/ – купи до 31 август с 15% отстъпка</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>249</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/e4/fp/e41a52ce5b8f56dc892f87c7e0d51e6e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/cf/fp/cf2dd9106d988f2d4c4444e227302206.jpg</t>
         </is>
       </c>
     </row>
@@ -2179,10 +2007,8 @@
           <t>Бмх</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="C88" t="n">
+        <v>250</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2192,1481 +2018,1333 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Градски велосипед</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+          <t>Велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>250</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/92/fp/927cc7e4970fe1b81dc2f56af6d90191.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/61/fp/61c5ca62cd6a1d83f1eb01b82fedad4a.jpg</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола RABENEICK-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+          <t>Колело РЕUGEOT. 24” , 18 скорости.</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>250</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/2b/fp/2be26912601688092400e03568fb06cf.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/44/fp/44366086ad32fabdbcaac6e72948dc6e.jpg</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Хидравлика-алуминиев велосипед 28 цола NISHIKI-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+          <t>Продавам велосипед Рокрайдер с подобрения</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>250</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/35/fp/35d60261403628a39c7c8b395d4a7622.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/0b/fp/0b8a549d0950aa4039e917a608cd60af.jpg</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Велосипед градски OBIKE-26цола.Бартер.</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>160</t>
-        </is>
+          <t>Продавам велосипед с 18 скорости ,бартер за лаптоп с камера и микрофон</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>250</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/e5/fp/e5c1468f5a90799fa452afa307596e70.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//37/fp/37bd87ab5d4018166499c98447050b32.jpg</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола BAISIKL-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+          <t>Алуминиев велосипед Ridgeback 28 цола</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>260</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/81/fp/8137cf7ca372ca8845d05d43ff113b9a.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/24/fp/2416d7c046e8bd65cf28c2b310c5d686.jpg</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Велосипед мъжки 26" LEADER WILD CAR</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+          <t>26 цолов алуминиев Велосипед Dirt- Street-Jump с 30дни гаранция</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>260</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/32/fp/322552ed96a9c32c2e37371b81ac0525.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/07/fp/0706422745caf249bc832c3ff0f57a3e.jpg</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Sintero Plus 2018 с гаранция</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>600</t>
-        </is>
+          <t>Английски алуминиев велосипед  Appollo FS26</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>260</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/4c/fp/4cb577e0f6404074ece560e509e72c68.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/f3/fp/f3bd79150713f68df0eaca9293588ab7.jpg</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>алуминиев велосипед 28 цола TRIUMPH-една година гаранция</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД B-TWIN ORIGINAL 500</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>270</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/75/fp/750b16d07d7dc94dd964636cfb23ac69.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/48/fp/4803796e9f073bc9bd1b09e9fbfeac8a.jpg</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>340</t>
-        </is>
+          <t>Градски алуминиев велосипед Ridgeback</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>280</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7f/fp/7fa591d2177a7f6ddc559ac279baf737.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/b7/fp/b7712206a87e3c89b223b0c73919278d.jpg</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед 28 цола</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>350</t>
-        </is>
+          <t>Американски велосипед GT ARROWHEAD</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>280</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/73/fp/73c24518d92cd38c520e1be5a3fde63c.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/52/fp/52b2be2c1f2ba2866d8450f1e719585b.jpg</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>350</t>
-        </is>
+          <t>алуминиев велосипед 28 цола BAISIKL-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>280</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/ec/fp/ec93c69f42103a42b51e781ccb8b094d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/81/fp/8137cf7ca372ca8845d05d43ff113b9a.jpg</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>ГРАДСКИ ВЕЛОСИПЕД KALKHOFF CITY SHOPPER</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД NERO 28-ЦОЛА</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>280</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/43/fp/439cd9eb0022a867012967a50072b928.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/49/fp/498e5bbc3285f736fb5baf2dbfef62fc.jpg</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Колело Батавус</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+          <t>ретро колело</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>280</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/be/fp/beb7a45e4b4d8bf5f24673c2f48e29c3.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/ec/fp/ec2c84d08847bc97f43184ab59dbf3eb.jpg</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>колело велосипед BATAVUS® Weekend</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+          <t>Велосипед Giant Escape</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>290</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/2d/fp/2df4786c6f3b20ae92a00270e047db98.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/32/fp/32ea2d5ca209a605d10e5f048391b0b1.jpg</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cannondele</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>680</t>
-        </is>
+          <t>Алуминиев велосипед/колело B-Twin 26"</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>290</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/ba/fp/ba1afd0ab95ada2f7480ebca50dd01d3.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/8b/fp/8b95cfde68e60f75bd68a79369eeda8c.jpg</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Планински бегач 26. HAWK 22 bleck line. Рамка 40 “. 26” цола</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>350</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД СГЪВАЕМ B-TWIN TILT 120 20-ЦОЛА</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>295</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/47/fp/479874964a7ad0c057b3b542316961a9.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/2b/fp/2bf8abbf86bcb0c01bc6d3b9b8fba539.jpg</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Продавам велосипед Sprint Sintero</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+          <t>Джет,ретро за извън бордов двигател финростъкло 3 броя</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>300</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/18/fp/180ca73cd894b65c9f3ad267080e8246.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/46/fp/46c815103d7ca6a9bfce677f78cef60a.jpg</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Колело Conway  28. 21 скорости.  Динамо вградено</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>360</t>
-        </is>
+          <t>Продавам алуминиев велосипед 26"</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>300</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/23/fp/23b4f61acdf838013173beffb67df714.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/15/fp/151329c21953a1b5229d546b1f38510b.jpg</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Класически велосипед SCOTT</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>160</t>
-        </is>
+          <t>Продавам велосипед РЕАКТОР ТОТЕМ 21 скорости 26"</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>300</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/79/fp/79aeeb1a245196ccb6a15f3739b941c9.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/47/fp/475229b606690e31b816b88322be4598.jpg</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+          <t>Продавам запазено колело</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>300</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/60/fp/60a697db700ce2a22d751a4dc7873d5b.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/18/fp/18420ba888752d14fdf6702dfc30d380.jpg</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Продавам 2 бр. Велосипеди</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>алуминиев велосипед 28 цола PEGASUS-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>300</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/28/fp/28f42ca8251736768a600fac96f37ed2.jpg</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Продавам 2 бр. Велосипеди</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>алуминиев велосипед 28 цола CALIFORNIA-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>320</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/65/fp/6578e95773650636f181f828f29b110e.jpg</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Продавам 2 бр. Велосипеди</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Алуминиев велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>340</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/be/fp/be5b0ba907c897639b42f039b9cda2ef.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7f/fp/7fa591d2177a7f6ddc559ac279baf737.jpg</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Колело Diamant</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>690</t>
-        </is>
+          <t>Алуминиев велосипед 28 цола</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>350</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/92/fp/9288252f47dd1a0ca1ed203b3c9a9584.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/73/fp/73c24518d92cd38c520e1be5a3fde63c.jpg</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
+          <t>Алуминиев велосипед 26 цола</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>350</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/4b/fp/4b54e94ea3ca6ca1c5dcb9057a63a1e9.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/ec/fp/ec93c69f42103a42b51e781ccb8b094d.jpg</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Колело РЕUGEOT. 24” , 18 скорости.</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+          <t>Планински бегач 26. HAWK 22 bleck line. Рамка 40 “. 26” цола</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>350</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/44/fp/44366086ad32fabdbcaac6e72948dc6e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/47/fp/479874964a7ad0c057b3b542316961a9.jpg</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Колело Giant NRS 1,26”</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
+          <t>алуминиев велосипед 28 цола HERCULES-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>360</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/04/fp/04b74f2ca91057d535224e3e1a20ca53.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/fb/fp/fb0589b6a874359f72054b018e4c09ea.jpg</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Колело Pegasus 26”, 21  скорости</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>Колело Conway  28. 21 скорости.  Динамо вградено</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>360</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/ab/fp/ab233c383eb90dc948c5d92e9f016c68.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/23/fp/23b4f61acdf838013173beffb67df714.jpg</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Продавам велосипед с 18 скорости или бартер за лаптоп с камера и микрофон</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>460</t>
-        </is>
+          <t>алуминиев велосипед 28 цола RABENEICK-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>380</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar//b7/fp/b73e543574f8e93f3b280eb92b337bd8.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/2b/fp/2be26912601688092400e03568fb06cf.jpg</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>градски велосипед</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>алуминиев велосипед 28 цола TRIUMPH-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>380</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/9d/fp/9dedc9c9f80b2b2c3f62ff1857ff3540.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/75/fp/750b16d07d7dc94dd964636cfb23ac69.jpg</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Велосипед Apollo Rich 26 цола</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД RIVERSIDE CIVERSIDE 320TR</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>390</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/39/fp/39e1c1a38c1afc1b4930dd0ab31bd219.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7e/fp/7ea34bead5088898bc142cf5bd8f6b98.jpg</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Гуми 28 цола nimbus700×32c kenda цената е за 2-те гуми</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+          <t>Колело pegasus avanti 28</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>390</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//da/fp/da81f5744ca833b088bbbfd2118af84e.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/17/fp/17c3297fef79d0ce968b5ae7873f4af0.jpg</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Калъф стойка за телефон монтаж за колело</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+          <t>Продавам велосипед Sprint Sintero</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>400</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//86/fp/861f50d5ecccf43f34e7b9b664224ac8.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/18/fp/180ca73cd894b65c9f3ad267080e8246.jpg</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Колело</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+          <t>Градско колело City bike. 28”. Shimano 28 скорости</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>400</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/03/fp/035cfb93deda57705fbe672790e066bb.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/65/fp/655c66aa98f01c32366e7002405175bd.jpg</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Хидравлика-алуминиев велосипед 28 цола NISHIKI-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>400</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/35/fp/35d60261403628a39c7c8b395d4a7622.jpg</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>18цолов детски велосипед с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+          <t>Градски велосипед 28цола</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>400</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/5c/fp/5c653da616a5ad68ce0e8ea9ac2c3e1d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/18/fp/18a5dc836f65140ee46f3e7ac76e9b96.jpg</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Btwin rockrider 25"</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>230</t>
-        </is>
+          <t>алуминиев велосипед 28 цола KALKHOFF-една година гаранция</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>420</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7f/fp/7fadf77edfc1059ddb6886bc3c1e0973.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/82/fp/82a0641a95ee4309e7b96e769fce251b.jpg</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Дан Хил Велосипед Giant Box Three</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>Електрически велосипед</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>450</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/8e/fp/8e3de7e8f6d2399ed729ea4b4ec5c218.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/53/fp/53983b72a173eb96188041242f3c00ed.jpg</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Страхотен велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>160</t>
-        </is>
+          <t>колело трек 28"</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>450</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/4e/fp/4e44dd70c0403518b9ce49be0beb8b84.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/2c/fp/2c0d7a46d0af6222b4f6faaed84088e7.jpg</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>ГОЛЯМ ИЗБОР НА ВЕЛОСИПЕДИ, ДИСПЛЕИ,ЗАРЯДНИ,БАТЕРИИ И ДР.ЗА ЕЛЕКТРИЧЕСКИ ВЕЛОСИПЕДИ</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>колело трек 28"</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>450</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//e3/fp/e372d75b8bd2adde6a85f31fcb04e1f6.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/2c/fp/2c0d7a46d0af6222b4f6faaed84088e7.jpg</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Велосипед Apollo Slant 17 ″</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+          <t>Продавам велосипед с 18 скорости или бартер за лаптоп с камера и микрофон</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>460</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/3f/fp/3fd9ae45c3b5c7753bab6a5338328862.jpg</t>
+          <t>https://cdn1.focus.bg/bazar//b7/fp/b73e543574f8e93f3b280eb92b337bd8.jpg</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>128</v>
+        <v>3</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Продавам велосипед Ultra PHANTOM/отлично състояние/ – купи до 31 август с 5% отстъпка</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+          <t>велосипед Cannondale USA</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>480</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/cf/fp/cf2dd9106d988f2d4c4444e227302206.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/33/fp/338062f566da65f604a110e8f9be9b2f.jpg</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед Ridgeback 28 цола</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
+          <t>Yamaha XPC 26  Електрическо колело</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>480</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/24/fp/2416d7c046e8bd65cf28c2b310c5d686.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/50/fp/5006bcf058c4170dec129fdca59bacc2.jpg</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Велосипед 24 цола Raleigh Ascender</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>135</t>
-        </is>
+          <t>Yamaha XPC 26  Електрическо колело</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>480</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/30/fp/306fae5cf84d2a1a423998655fe1fd0a.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/50/fp/5006bcf058c4170dec129fdca59bacc2.jpg</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>27цолов велосипед RALEIGH с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>149</t>
-        </is>
+          <t>Алуминиев велосипед 29 цола</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>490</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/88/fp/885add0c17e1b14f6fcc05497e8c3012.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/ae/fp/aee3c2518ab5d79be116c4ebc5f8386c.jpg</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>26 цолов алуминиев Велосипед Dirt- Street-Jump с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
+          <t>колело велосипед BATAVUS® Weekend</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>500</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/07/fp/0706422745caf249bc832c3ff0f57a3e.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/2d/fp/2df4786c6f3b20ae92a00270e047db98.jpg</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ретро колело</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+          <t>Колело</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>500</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/ec/fp/ec2c84d08847bc97f43184ab59dbf3eb.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/03/fp/035cfb93deda57705fbe672790e066bb.jpg</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Велосипед 26 цола</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>ГРАДСКИ ВЕЛОСИПЕД ELECTRA LOFT 7D 2020г. модел 28-цола</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>540</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/45/fp/45b3f03fee98f75b141a73cc01cab67d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/6b/fp/6badad64d8946a06936635cc00e8e959.jpg</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Карбонов велосипед 26 цола Giant</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>730</t>
-        </is>
+          <t>Велосипед</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>550</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/70/fp/708663eb2f6a13747ac56a55ba91fb4f.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/85/fp/85cb90dd4c1e76ce5611dd3d371e804e.jpg</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Карбонов велосипед 26 цола Trek</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>730</t>
-        </is>
+          <t>Колело SERIOUS. ROCKVILE. 27,5 “. Рамка L.  27 ск.</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>580</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/e8/fp/e82cb83fc48f74a56361a08d450660aa.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/e5/fp/e58ef5fe4728d5855318b7e3f0abe3c2.jpg</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Велосипед</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+          <t>Колело 26 Bike. KONA. SCRAP</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>590</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/99/fp/99319cb3fe4ad0c112f975d6ec23f2fc.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/7a/fp/7a71ed3f09c5a125a90b1a8ab2cc0153.jpg</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Велосипед Gemini Outrider</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>160</t>
-        </is>
+          <t>Sintero Plus 2018 с гаранция</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>600</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/0c/fp/0c5258b46ca3689f6fbc05bfb21e6648.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/4c/fp/4cb577e0f6404074ece560e509e72c68.jpg</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Велосипед Giant Escape</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>290</t>
-        </is>
+          <t>Градски велосипед</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>600</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/32/fp/32ea2d5ca209a605d10e5f048391b0b1.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/8b/fp/8b79fac85cd3abde9b9057ed733d6c0d.jpg</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Велосипед Аполо Рефлекс/ Apolo Reflex 20 цола</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
+          <t>Xiaomi M365 Гуми външни,вътрешни и плътни 8 1/2 х 2 Високо качество!</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>650</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7c/fp/7c11da05fa04a8546bf3a713f2f6d474.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/10/fp/102f0aaa28d8eeb233f9db70f354d4e9.jpg</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>141</v>
+        <v>51</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Велосипед САРАЦЕН Роял</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>215</t>
-        </is>
+          <t>Велосипед Specialised</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>650</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/d6/fp/d6590de5704d3ee70c528241a4ff0f78.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/b1/fp/b1b54305233d78dedb6f96d170c89ad0.jpg</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>142</v>
+        <v>50</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Продавам велосипед с 18 скорости ,бартер за лаптоп с камера и микрофон</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+          <t>Велосипед Cannondele</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>680</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar//37/fp/37bd87ab5d4018166499c98447050b32.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/a6/fp/a69ea0a8fb5b84dd62bdc65560b9a5f4.jpg</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Джет,ретро за извън бордов двигател финростъкло 3 броя</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>Cannondele</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>680</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/46/fp/46c815103d7ca6a9bfce677f78cef60a.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/ba/fp/ba1afd0ab95ada2f7480ebca50dd01d3.jpg</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+          <t>Колело Diamant</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>690</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/92/fp/9288252f47dd1a0ca1ed203b3c9a9584.jpg</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>18цолов детски велосипед с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+          <t>Немско дамско колело Diamont</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>690</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/5c/fp/5c653da616a5ad68ce0e8ea9ac2c3e1d.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/72/fp/7298c5f95b5176e1302320c299736ab6.jpg</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Дан Хил Велосипед Giant Box Three</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
+          <t>Колело Giant NRS 1,26”</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>700</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/44/fp/443ec0dfa7302337885def175973ec1a.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/04/fp/04b74f2ca91057d535224e3e1a20ca53.jpg</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>18цолов велосипед BMX Rhino с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+          <t>Карбонов велосипед 26 цола Trek</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>730</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/fb/fp/fbfa74f58a03b972c26d3bf5f6e18c11.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/e8/fp/e82cb83fc48f74a56361a08d450660aa.jpg</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>18цолов велосипед Lark с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
+          <t>Карбонов велосипед 26 цола Giant</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>730</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/62/fp/62cb140e5648916e2d4d5aa99b2bfa56.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/70/fp/708663eb2f6a13747ac56a55ba91fb4f.jpg</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>20цолов велосипед Calypso с 30дни гаранция</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+          <t>Велосипед хибрид Giant roam xr 2</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>800</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/17/fp/179ac9264931faa480b302fc92bc810e.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/b9/fp/b9f9e4dc28d611b80ab8b03c6b4883dc.jpg</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Продавам велосипед РЕАКТОР ТОТЕМ 21 скорости 26"</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
+          <t>Колело miutin 26”</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>800</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/47/fp/475229b606690e31b816b88322be4598.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/92/fp/9206f82ee0561a90e053590f484a1926.jpg</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>151</v>
+        <v>65</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Градски, шосеен велосипед - city camouflage</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
+          <t>Карбонов велосипед  Specialized tarmac. 28 цола</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>800</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/28/fp/281d4b2a6a820a98e6428d0a6c3be7b9.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/24/fp/2496e26ad1d456b890fedf9813cc9731.jpg</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Алуминиев велосипед 29 цола</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>490</t>
-        </is>
+          <t>Немско колело Telefunken с динамо</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>900</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/ae/fp/aee3c2518ab5d79be116c4ebc5f8386c.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/3a/fp/3a0cf2efb71ee0068f8b19cfa8d26f3c.jpg</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Немско дамско колело Diamont</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>690</t>
-        </is>
+          <t>Алуминиев велосипед Bulls 29</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>900</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/72/fp/7298c5f95b5176e1302320c299736ab6.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/46/fp/46dddbdc55bf343f74ca15663d4fff1c.jpg</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Колело 26 Bike. KONA. SCRAP</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>590</t>
-        </is>
+          <t>Градски, шосеен велосипед - city camouflage</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>999</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/7a/fp/7a71ed3f09c5a125a90b1a8ab2cc0153.jpg</t>
+          <t>https://cdn5.focus.bg/bazar/28/fp/281d4b2a6a820a98e6428d0a6c3be7b9.jpg</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Немско колело Telefunken с динамо</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>900</t>
-        </is>
+          <t>Велосипед Nirve Fairfaxт</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>999</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/3a/fp/3a0cf2efb71ee0068f8b19cfa8d26f3c.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//59/fp/592cd39b171d5836c336b79f324a2a17.jpg</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Колело pegasus avanti 28</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>390</t>
-        </is>
+          <t>octane one street dirt jump bike</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>1000</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>https://cdn5.focus.bg/bazar/17/fp/17c3297fef79d0ce968b5ae7873f4af0.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/c3/fp/c3c20bd0d19b39fe50739f83ad0c4ac9.jpg</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Две капли 26” оборудвани с гуми + бонус</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+          <t>Avenue spirit 1000</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>1300</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/5f/fp/5f43794ab809428bb372a605143f005f.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/10/fp/106de41fa4f6c84eaa01448a0a5abbf1.jpg</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>158</v>
+        <v>10</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Велосипед Omega Rolan L Чисто Ново колело 26”</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>530</t>
-        </is>
+          <t>Ел. колело, електрическо колело, електро колело</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>1450</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/52/fp/52ac271391d6fb1b4c722cef671e6d20.jpg</t>
+          <t>https://cdn5.focus.bg/bazar//42/fp/4205ae8e47ce0f1e05d60ddbfc015098.jpg</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Yamaha XPC 26  Електрическо колело</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+          <t>Немски електрически велосипед Kreidler 28</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>1500</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/50/fp/5006bcf058c4170dec129fdca59bacc2.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/c2/fp/c2d17836e616d2cd4120dcbfa1f9e4a1.jpg</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Продавам велосипед Ultra PHANTOM/отлично състояние/ – купи до 31 август с 5% отстъпка</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>199</t>
-        </is>
+          <t>Велосипед шосеен Canyon</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>1600</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>https://cdn1.focus.bg/bazar/cf/fp/cf2dd9106d988f2d4c4444e227302206.jpg</t>
+          <t>https://cdn1.focus.bg/bazar/aa/fp/aa3095cb1837ba62cbec39a400ca9ca4.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>